<commit_message>
heating technology size is added to the *main heating technology* (only) and collected. This is done for building initialization, new construction, and heating technology replacement.
Besides, a bug in the previous code is fixed: the size was only calculated with useful energy demand and efficiency info was missing. Now it is added.
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Parameter_HeatingTechnology_SizeQuantile.xlsx
+++ b/projects/test_building/input/Parameter_HeatingTechnology_SizeQuantile.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CBA650-1E0E-CE4F-8839-C5FB40FF2002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7036DA3A-4B57-0941-9456-2AE129F037FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="22260" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28580" yWindow="2180" windowWidth="22260" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="4">
   <si>
     <t>unit</t>
   </si>
@@ -87,8 +87,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C30" totalsRowShown="0">
-  <autoFilter ref="A1:C30" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C26" totalsRowShown="0">
+  <autoFilter ref="A1:C26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id_heating_technology"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="unit"/>
@@ -361,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -495,7 +495,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>29</v>
+        <v>210</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
@@ -506,7 +506,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
@@ -517,7 +517,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
@@ -528,7 +528,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
@@ -539,7 +539,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>211</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>212</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
@@ -561,7 +561,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>213</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
@@ -572,7 +572,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
@@ -583,7 +583,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
@@ -594,7 +594,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
@@ -605,7 +605,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
@@ -616,7 +616,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
@@ -627,7 +627,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
@@ -638,7 +638,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>
@@ -649,56 +649,12 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
         <v>3</v>
       </c>
       <c r="C26">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>44</v>
-      </c>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>45</v>
-      </c>
-      <c r="B28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>46</v>
-      </c>
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>50</v>
-      </c>
-      <c r="B30" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30">
         <v>0.25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
heating technology size --> 10% quantile
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Parameter_HeatingTechnology_SizeQuantile.xlsx
+++ b/projects/test_building/input/Parameter_HeatingTechnology_SizeQuantile.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7036DA3A-4B57-0941-9456-2AE129F037FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4871A591-5575-B04A-91B5-7444140566E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28580" yWindow="2180" windowWidth="22260" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -364,7 +364,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -391,7 +391,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -402,7 +402,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -413,7 +413,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -424,7 +424,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -435,7 +435,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -446,7 +446,7 @@
         <v>3</v>
       </c>
       <c r="C7">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -457,7 +457,7 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -468,7 +468,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -479,7 +479,7 @@
         <v>3</v>
       </c>
       <c r="C10">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -490,7 +490,7 @@
         <v>3</v>
       </c>
       <c r="C11">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -501,7 +501,7 @@
         <v>3</v>
       </c>
       <c r="C12">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -512,7 +512,7 @@
         <v>3</v>
       </c>
       <c r="C13">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -523,7 +523,7 @@
         <v>3</v>
       </c>
       <c r="C14">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -534,7 +534,7 @@
         <v>3</v>
       </c>
       <c r="C15">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -545,7 +545,7 @@
         <v>3</v>
       </c>
       <c r="C16">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -556,7 +556,7 @@
         <v>3</v>
       </c>
       <c r="C17">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -567,7 +567,7 @@
         <v>3</v>
       </c>
       <c r="C18">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -578,7 +578,7 @@
         <v>3</v>
       </c>
       <c r="C19">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -589,7 +589,7 @@
         <v>3</v>
       </c>
       <c r="C20">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -600,7 +600,7 @@
         <v>3</v>
       </c>
       <c r="C21">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -611,7 +611,7 @@
         <v>3</v>
       </c>
       <c r="C22">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -622,7 +622,7 @@
         <v>3</v>
       </c>
       <c r="C23">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -633,7 +633,7 @@
         <v>3</v>
       </c>
       <c r="C24">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -644,7 +644,7 @@
         <v>3</v>
       </c>
       <c r="C25">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -655,7 +655,7 @@
         <v>3</v>
       </c>
       <c r="C26">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>